<commit_message>
change output format, reshape mlst tables
</commit_message>
<xml_diff>
--- a/EFSA_output/merged_results.xlsx
+++ b/EFSA_output/merged_results.xlsx
@@ -629,39 +629,39 @@
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
+          <t>Serotype</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>SerotypePrediction_Software</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
           <t>QualityCheck</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Results</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>Serotype</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>SerotypePrediction_Software</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Strain0013</t>
+          <t>Strain0016</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C2" t="n">
         <v>0.93</v>
       </c>
       <c r="D2" t="n">
-        <v>320054819</v>
+        <v>417855250</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>161.22</v>
+        <v>209.23</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="L2" t="n">
-        <v>329009</v>
+        <v>359519</v>
       </c>
       <c r="M2" t="n">
         <v>0.9</v>
@@ -701,28 +701,28 @@
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>2848</v>
+        <v>2883</v>
       </c>
       <c r="Q2" t="n">
-        <v>70367.53999999999</v>
+        <v>94022.58</v>
       </c>
       <c r="R2" t="n">
-        <v>2885069</v>
+        <v>2914700</v>
       </c>
       <c r="S2" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="T2" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="U2" t="n">
-        <v>0.3792</v>
+        <v>0.3789</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>435270</v>
+        <v>480313</v>
       </c>
       <c r="X2" t="b">
         <v>1</v>
@@ -801,202 +801,140 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Strain0014</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Strain02</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>147</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="D3" t="n">
+        <v>616082012</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>Error processing sample</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>115.72</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>salmonella enterica</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>103</v>
+      </c>
+      <c r="L3" t="n">
+        <v>400565</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="N3" t="n">
+        <v>99.69</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="P3" t="n">
+        <v>4822</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>84731.42</v>
+      </c>
+      <c r="R3" t="n">
+        <v>4999154</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="T3" t="n">
+        <v>59</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.5205</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>773613</v>
+      </c>
+      <c r="X3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AF3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>5</v>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>4.1.5</t>
+        </is>
+      </c>
+      <c r="AI3" t="n">
+        <v>10</v>
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>mlst</t>
         </is>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>abricate</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>abricate/abricate.csv</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Dublin</t>
         </is>
       </c>
       <c r="AN3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>SeqSero2</t>
         </is>
       </c>
       <c r="AO3" t="inlineStr">
@@ -1013,130 +951,192 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>136</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="D4" t="n">
-        <v>417855250</v>
+          <t>Strain0014</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Error processing sample</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>209.23</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>listeria monocytogenes</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>120</v>
-      </c>
-      <c r="L4" t="n">
-        <v>359519</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="N4" t="n">
-        <v>99.45</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2883</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>94022.58</v>
-      </c>
-      <c r="R4" t="n">
-        <v>2914700</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="T4" t="n">
-        <v>31</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.3789</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>480313</v>
-      </c>
-      <c r="X4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>4</v>
-      </c>
-      <c r="AF4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>1</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>4.1.5</t>
-        </is>
-      </c>
-      <c r="AI4" t="n">
-        <v>451</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>mlst</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>abricate</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>abricate/abricate.csv</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AM4" t="inlineStr">
@@ -1163,17 +1163,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" t="n">
         <v>0.92</v>
       </c>
       <c r="D5" t="n">
-        <v>554653013</v>
+        <v>663403630</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -1181,7 +1181,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>99.90000000000001</v>
+        <v>124.39</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -1198,34 +1198,34 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="L5" t="n">
-        <v>223534</v>
+        <v>401772</v>
       </c>
       <c r="M5" t="n">
         <v>0.87</v>
       </c>
       <c r="N5" t="n">
-        <v>99.69</v>
+        <v>99.65000000000001</v>
       </c>
       <c r="O5" t="n">
         <v>0.08</v>
       </c>
       <c r="P5" t="n">
-        <v>4684</v>
+        <v>4678</v>
       </c>
       <c r="Q5" t="n">
-        <v>73805.21000000001</v>
+        <v>110817.66</v>
       </c>
       <c r="R5" t="n">
-        <v>4871144</v>
+        <v>4875977</v>
       </c>
       <c r="S5" t="n">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="T5" t="n">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="U5" t="n">
         <v>0.5209</v>
@@ -1234,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>727607</v>
+        <v>738266</v>
       </c>
       <c r="X5" t="b">
         <v>1</v>
@@ -1258,13 +1258,13 @@
         <v>1</v>
       </c>
       <c r="AE5" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AF5" t="b">
         <v>1</v>
       </c>
       <c r="AG5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
@@ -1291,29 +1291,29 @@
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Dublin</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>SeqSero2</t>
         </is>
       </c>
       <c r="AO5" t="inlineStr">
         <is>
-          <t>Dublin</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AP5" t="inlineStr">
         <is>
-          <t>SeqSero2</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1323,11 +1323,11 @@
         <v>0.92</v>
       </c>
       <c r="D6" t="n">
-        <v>616082012</v>
+        <v>554653013</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Error processing sample</t>
+          <t>Salmonella</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>115.72</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -1348,10 +1348,10 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="L6" t="n">
-        <v>400565</v>
+        <v>223534</v>
       </c>
       <c r="M6" t="n">
         <v>0.87</v>
@@ -1363,28 +1363,28 @@
         <v>0.08</v>
       </c>
       <c r="P6" t="n">
-        <v>4822</v>
+        <v>4684</v>
       </c>
       <c r="Q6" t="n">
-        <v>84731.42</v>
+        <v>73805.21000000001</v>
       </c>
       <c r="R6" t="n">
-        <v>4999154</v>
+        <v>4871144</v>
       </c>
       <c r="S6" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="T6" t="n">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="U6" t="n">
-        <v>0.5205</v>
+        <v>0.5209</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>773613</v>
+        <v>727607</v>
       </c>
       <c r="X6" t="b">
         <v>1</v>
@@ -1408,13 +1408,13 @@
         <v>1</v>
       </c>
       <c r="AE6" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AF6" t="b">
         <v>1</v>
       </c>
       <c r="AG6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
@@ -1441,47 +1441,47 @@
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Dublin</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>SeqSero2</t>
         </is>
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>Dublin</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AP6" t="inlineStr">
         <is>
-          <t>SeqSero2</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain0013</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C7" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="D7" t="n">
-        <v>663403630</v>
+        <v>320054819</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Salmonella</t>
+          <t>Error processing sample</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1490,51 +1490,51 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>124.39</v>
+        <v>161.22</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>salmonella enterica</t>
+          <t>listeria monocytogenes</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="L7" t="n">
-        <v>401772</v>
+        <v>329009</v>
       </c>
       <c r="M7" t="n">
-        <v>0.87</v>
+        <v>0.9</v>
       </c>
       <c r="N7" t="n">
-        <v>99.65000000000001</v>
+        <v>99.45</v>
       </c>
       <c r="O7" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>4678</v>
+        <v>2848</v>
       </c>
       <c r="Q7" t="n">
-        <v>110817.66</v>
+        <v>70367.53999999999</v>
       </c>
       <c r="R7" t="n">
-        <v>4875977</v>
+        <v>2885069</v>
       </c>
       <c r="S7" t="n">
         <v>0.04</v>
       </c>
       <c r="T7" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="U7" t="n">
-        <v>0.5209</v>
+        <v>0.3792</v>
       </c>
       <c r="V7" t="n">
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>738266</v>
+        <v>435270</v>
       </c>
       <c r="X7" t="b">
         <v>1</v>
@@ -1558,13 +1558,13 @@
         <v>1</v>
       </c>
       <c r="AE7" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="AF7" t="b">
         <v>1</v>
       </c>
       <c r="AG7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="AI7" t="n">
-        <v>10</v>
+        <v>451</v>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
@@ -1601,12 +1601,12 @@
       </c>
       <c r="AO7" t="inlineStr">
         <is>
-          <t>Dublin</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AP7" t="inlineStr">
         <is>
-          <t>SeqSero2</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1824,7 +1824,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1906,7 +1906,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1988,7 +1988,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2070,7 +2070,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2152,7 +2152,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2175,34 +2175,34 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1133</v>
+        <v>28</v>
       </c>
       <c r="H7" t="n">
-        <v>1133</v>
+        <v>28</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>ttc</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>ctc</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>16S_rrsD_1133_g</t>
+          <t>acrB_28_l</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>16S_rrsD_1133_g</t>
+          <t>acrB_28_l</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>r.1133A&gt;G</t>
+          <t>p.F28L</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -2212,29 +2212,29 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>16S_rrsD</t>
+          <t>acrB</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>f</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>l</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ttc&gt;ctc</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2257,34 +2257,34 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="H8" t="n">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>ttc</t>
+          <t>cta</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ctc</t>
+          <t>cca</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>acrB_28_l</t>
+          <t>acrB_40_p</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>acrB_28_l</t>
+          <t>acrB_40_p</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>p.F28L</t>
+          <t>p.L40P</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -2299,24 +2299,24 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>f</t>
+          <t>l</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>ttc&gt;ctc</t>
+          <t>cta&gt;cca</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2339,34 +2339,34 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>40</v>
+        <v>868</v>
       </c>
       <c r="H9" t="n">
-        <v>40</v>
+        <v>868</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>cta</t>
+          <t>agc</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>cca</t>
+          <t>aac</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>acrB_40_p</t>
+          <t>gyrA_868_n</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>acrB_40_p</t>
+          <t>gyrA_868_n</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>p.L40P</t>
+          <t>p.S868N</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -2376,29 +2376,29 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>acrB</t>
+          <t>gyrA</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>s</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>p</t>
+          <t>n</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>cta&gt;cca</t>
+          <t>agc&gt;aac</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2421,34 +2421,34 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>868</v>
+        <v>648</v>
       </c>
       <c r="H10" t="n">
-        <v>868</v>
+        <v>648</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>agc</t>
+          <t>cag</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>aac</t>
+          <t>ctg</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>gyrA_868_n</t>
+          <t>parC_648_l</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>gyrA_868_n</t>
+          <t>parC_648_l</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>p.S868N</t>
+          <t>p.Q648L</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -2458,29 +2458,29 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>gyrA</t>
+          <t>parC</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>s</t>
+          <t>q</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>n</t>
+          <t>l</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>agc&gt;aac</t>
+          <t>cag&gt;ctg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain02</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2503,34 +2503,34 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>648</v>
+        <v>9</v>
       </c>
       <c r="H11" t="n">
-        <v>648</v>
+        <v>9</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>cag</t>
+          <t>acc</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ctg</t>
+          <t>ccc</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>parC_648_l</t>
+          <t>pmrB_9_p</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>parC_648_l</t>
+          <t>pmrB_9_p</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>p.Q648L</t>
+          <t>p.T9P</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -2540,29 +2540,29 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>parC</t>
+          <t>pmrB</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>q</t>
+          <t>t</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>p</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>cag&gt;ctg</t>
+          <t>acc&gt;ccc</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Strain01</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2585,34 +2585,34 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="H12" t="n">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>acc</t>
+          <t>c</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>ccc</t>
+          <t>t</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>pmrB_9_p</t>
+          <t>16S_rrsD_92_t</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>pmrB_9_p</t>
+          <t>16S_rrsD_92_t</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>p.T9P</t>
+          <t>r.92C&gt;T</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -2622,29 +2622,29 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>pmrB</t>
+          <t>16S_rrsD</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>-</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>p</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>acc&gt;ccc</t>
+          <t>-</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2667,10 +2667,10 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>92</v>
+        <v>1005</v>
       </c>
       <c r="H13" t="n">
-        <v>92</v>
+        <v>1005</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -2679,22 +2679,22 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>g</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>16S_rrsD_92_t</t>
+          <t>16S_rrsD_1005_g</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>16S_rrsD_92_t</t>
+          <t>16S_rrsD_1005_g</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>r.92C&gt;T</t>
+          <t>r.1005C&gt;G</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -2726,7 +2726,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2749,34 +2749,34 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="H14" t="n">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>t</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>a</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>16S_rrsD_1005_g</t>
+          <t>16S_rrsD_1006_a</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>16S_rrsD_1005_g</t>
+          <t>16S_rrsD_1006_a</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>r.1005C&gt;G</t>
+          <t>r.1006T&gt;A</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -2808,7 +2808,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2831,10 +2831,10 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="H15" t="n">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -2848,17 +2848,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>16S_rrsD_1006_a</t>
+          <t>16S_rrsD_1007_a</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>16S_rrsD_1006_a</t>
+          <t>16S_rrsD_1007_a</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>r.1006T&gt;A</t>
+          <t>r.1007T&gt;A</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -2890,7 +2890,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2913,34 +2913,34 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>1007</v>
+        <v>1022</v>
       </c>
       <c r="H16" t="n">
-        <v>1007</v>
+        <v>1022</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
           <t>t</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>16S_rrsD_1007_a</t>
+          <t>16S_rrsD_1022_t</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>16S_rrsD_1007_a</t>
+          <t>16S_rrsD_1022_t</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>r.1007T&gt;A</t>
+          <t>r.1022G&gt;T</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -2972,7 +2972,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2995,34 +2995,34 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>1022</v>
+        <v>1133</v>
       </c>
       <c r="H17" t="n">
-        <v>1022</v>
+        <v>1133</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
           <t>g</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>16S_rrsD_1022_t</t>
+          <t>16S_rrsD_1133_g</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>16S_rrsD_1022_t</t>
+          <t>16S_rrsD_1133_g</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>r.1022G&gt;T</t>
+          <t>r.1133A&gt;G</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -3054,7 +3054,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3136,7 +3136,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3218,7 +3218,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3300,7 +3300,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Strain02</t>
+          <t>Strain03</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3464,7 +3464,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -3546,7 +3546,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3628,7 +3628,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -3710,7 +3710,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3792,7 +3792,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3874,7 +3874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -3956,7 +3956,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4038,7 +4038,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4120,7 +4120,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -4202,7 +4202,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -4284,7 +4284,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Strain03</t>
+          <t>Strain01</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -4374,7 +4374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4390,73 +4390,398 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Gene</t>
+          <t>ST</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ST</t>
+          <t>bglA</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ldh</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dat</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>abcZ</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>lhkA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>cat</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>dapE</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>thrA</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>hisD</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>sucA</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>hemD</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>dnaN</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>aroC</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>purE</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>cat</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>10</v>
+          <t>Strain0016</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>451</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>dapE</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>21</v>
+          <t>Strain02</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>abcZ</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>7</v>
+          <t>Strain03</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>dat</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
+          <t>Strain01</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -4465,1057 +4790,77 @@
           <t>Strain0013</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>lhkA</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ldh</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>bglA</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>bglA</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ldh</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>dat</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>abcZ</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>lhkA</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>cat</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>dapE</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>dnaN</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>sucA</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>hemD</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>thrA</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>aroC</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>hisD</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>purE</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>thrA</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>hisD</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>sucA</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>hemD</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>dnaN</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>aroC</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>purE</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>thrA</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>dnaN</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>sucA</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>purE</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>hemD</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>aroC</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>hisD</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>cat</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
+      <c r="B6" t="n">
+        <v>451</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>dapE</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>21</t>
         </is>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>abcZ</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>dat</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>lhkA</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>ldh</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Strain0013</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>bglA</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>bglA</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>ldh</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>dat</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>abcZ</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>lhkA</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>cat</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Strain0016</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>dapE</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>dnaN</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>sucA</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>hemD</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>thrA</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>aroC</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>hisD</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Strain01</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>purE</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>thrA</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>hisD</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>sucA</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>hemD</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>dnaN</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>aroC</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Strain02</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>purE</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>thrA</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>dnaN</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>sucA</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>purE</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>hemD</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>aroC</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Strain03</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>hisD</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>6</t>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>